<commit_message>
pandas, numphy workings to clean data
</commit_message>
<xml_diff>
--- a/modified.xlsx
+++ b/modified.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -367,6 +367,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Area Code</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>First</t>
@@ -379,33 +384,23 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>City</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>City</t>
+          <t>State</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>State</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Area Code</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Extra</t>
+          <t>Income</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>8074</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -419,29 +414,21 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>120 jefferson st.</t>
+          <t>Riverside</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Riverside</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
           <t xml:space="preserve"> NJ</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>8074</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="F2" t="n">
         <v>45000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>9119</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -455,33 +442,25 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>220 hobo Av.</t>
+          <t>Phila</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Phila</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
           <t xml:space="preserve"> PA</t>
         </is>
       </c>
-      <c r="G3" t="n">
-        <v>9119</v>
-      </c>
-      <c r="H3" t="n">
+      <c r="F3" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>8075</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>John "Da Man"</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -491,29 +470,21 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>120 Jefferson St.</t>
+          <t>Riverside</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Riverside</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
           <t xml:space="preserve"> NJ</t>
         </is>
       </c>
-      <c r="G4" t="n">
-        <v>8075</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="F4" t="n">
         <v>120000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>91234</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -527,61 +498,53 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>7452 Terrace "At the Plaza" road</t>
+          <t>SomeTown</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>SomeTown</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
           <t>SD</t>
         </is>
       </c>
-      <c r="G5" t="n">
-        <v>91234</v>
-      </c>
-      <c r="H5" t="n">
+      <c r="F5" t="n">
         <v>90000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr"/>
+        <v>298</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>Blankman</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>SomeTown</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>SomeTown</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
           <t xml:space="preserve"> SD</t>
         </is>
       </c>
-      <c r="G6" t="n">
-        <v>298</v>
-      </c>
-      <c r="H6" t="n">
+      <c r="F6" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Joan "Danger", Anne</t>
+          <t>Joan</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -591,23 +554,15 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>9th, at Terrace plc</t>
+          <t>Desert City</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Desert City</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
           <t>CO</t>
         </is>
       </c>
-      <c r="G7" t="n">
-        <v>123</v>
-      </c>
-      <c r="H7" t="n">
+      <c r="F7" t="n">
         <v>68000</v>
       </c>
     </row>

</xml_diff>